<commit_message>
Final simulation ready to roll
</commit_message>
<xml_diff>
--- a/avg throughput.xlsx
+++ b/avg throughput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://antares3-my.sharepoint.com/personal/martonm_antaressolutions_com_au/Documents/Documents/Uni/COSC2673 Computational Machine Learning/Assignments/Assignment 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\RMIT\2022\COSC2793 - Computational Machine Learning\Assignment02\CML-Assign2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65404B31-F14B-4744-87DC-787FF8958F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F048E427-13F0-46D9-8F2A-8960D44B2961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="15" windowWidth="28215" windowHeight="17265" xr2:uid="{77E8CC37-C84C-49FF-AEED-C13EBEDEEC46}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{77E8CC37-C84C-49FF-AEED-C13EBEDEEC46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>minute</t>
   </si>
@@ -80,6 +80,45 @@
   </si>
   <si>
     <t>Overall average throughput per minute = 35.45 cars per minute</t>
+  </si>
+  <si>
+    <t>vph</t>
+  </si>
+  <si>
+    <t>east_west</t>
+  </si>
+  <si>
+    <t>east_south</t>
+  </si>
+  <si>
+    <t>east_north</t>
+  </si>
+  <si>
+    <t>west_east</t>
+  </si>
+  <si>
+    <t>west_south</t>
+  </si>
+  <si>
+    <t>west_north</t>
+  </si>
+  <si>
+    <t>south_north</t>
+  </si>
+  <si>
+    <t>south_west</t>
+  </si>
+  <si>
+    <t>south_east</t>
+  </si>
+  <si>
+    <t>north_south</t>
+  </si>
+  <si>
+    <t>north_east</t>
+  </si>
+  <si>
+    <t>north_west</t>
   </si>
 </sst>
 </file>
@@ -149,12 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,27 +512,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -533,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -574,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -615,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -656,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -697,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -738,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -779,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -820,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -861,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -902,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -943,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -984,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1025,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1066,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1107,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1148,7 +1188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1189,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1230,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1271,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1312,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1353,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -1406,8 +1446,99 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="5">
+        <f>B22*60</f>
+        <v>573</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" ref="C23:M23" si="1">C22*60</f>
+        <v>9</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="1"/>
+        <v>189</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>741</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="1"/>
+        <v>339</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>